<commit_message>
updated on 11th of july
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t xml:space="preserve">Maandag</t>
   </si>
@@ -67,7 +67,28 @@
     <t xml:space="preserve">ROS Leren/ Praten over research questions</t>
   </si>
   <si>
+    <t xml:space="preserve">Geo BBQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annet Weekend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly Review doen, RQT graphs van SSL Slam en ORB Slam maken, ROS doorspitten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onderzoeksvraag maken, Carlas en Robert Update sturen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Progress Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI Spelen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naar Ouders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre Vakantie Weekend</t>
   </si>
   <si>
     <t xml:space="preserve">Vakantie</t>
@@ -91,7 +112,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,10 +134,9 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +147,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD0CECE"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE16173"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -192,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,11 +250,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -265,7 +298,7 @@
       <rgbColor rgb="FFFFF2CC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFE16173"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -313,10 +346,10 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="21.44"/>
   </cols>
@@ -419,8 +452,12 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="0" t="n">
         <f aca="false">I4+1</f>
@@ -432,15 +469,23 @@
         <f aca="false">A5+7</f>
         <v>44382</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I6" s="0" t="n">
         <f aca="false">I5+1</f>
         <v>5</v>
@@ -456,7 +501,9 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="7"/>
       <c r="I7" s="0" t="n">
         <f aca="false">I6+1</f>
@@ -468,23 +515,23 @@
         <f aca="false">A7+7</f>
         <v>44396</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>16</v>
+      <c r="B8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H8" s="7"/>
     </row>
@@ -493,20 +540,20 @@
         <f aca="false">A8+7</f>
         <v>44403</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>16</v>
+      <c r="B9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -516,20 +563,20 @@
         <f aca="false">A9+7</f>
         <v>44410</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>16</v>
+      <c r="B10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -677,7 +724,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="9" t="n">
+      <c r="I19" s="11" t="n">
         <f aca="false">I18+1</f>
         <v>14</v>
       </c>

</xml_diff>